<commit_message>
split words columns and use Chinese
</commit_message>
<xml_diff>
--- a/data/words/v1/动词词库.xlsx
+++ b/data/words/v1/动词词库.xlsx
@@ -21,58 +21,58 @@
     <t>动词</t>
   </si>
   <si>
-    <t>及物+动词-心理活动</t>
-  </si>
-  <si>
-    <t>及物+动词-趋向</t>
-  </si>
-  <si>
-    <t>及物+动词-开始</t>
-  </si>
-  <si>
-    <t>及物+动词-结束</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-手臂-中性</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-手臂-亲切</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-手臂-消极</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-手臂-清扫</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-眼部-中性</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-眼部-贬义</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-耳部</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-嘴部</t>
-  </si>
-  <si>
-    <t>及物+名词-动作-身体</t>
-  </si>
-  <si>
-    <t>及物+名词-心情</t>
-  </si>
-  <si>
-    <t>及物+名词-存在</t>
-  </si>
-  <si>
-    <t>及物+名词-判断</t>
-  </si>
-  <si>
-    <t>及物+名词-意愿</t>
-  </si>
-  <si>
-    <t>及物+名词-趋向</t>
+    <t>及物_动词-心理活动</t>
+  </si>
+  <si>
+    <t>及物_动词-趋向</t>
+  </si>
+  <si>
+    <t>及物_动词-开始</t>
+  </si>
+  <si>
+    <t>及物_动词-结束</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-手臂-中性</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-手臂-亲切</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-手臂-消极</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-手臂-清扫</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-眼部-中性</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-眼部-贬义</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-耳部</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-嘴部</t>
+  </si>
+  <si>
+    <t>及物_名词-动作-身体</t>
+  </si>
+  <si>
+    <t>及物_名词-心情</t>
+  </si>
+  <si>
+    <t>及物_名词-存在</t>
+  </si>
+  <si>
+    <t>及物_名词-判断</t>
+  </si>
+  <si>
+    <t>及物_名词-意愿</t>
+  </si>
+  <si>
+    <t>及物_名词-趋向</t>
   </si>
   <si>
     <t>不及物-存在变化-生命</t>
@@ -707,12 +707,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -735,7 +735,60 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -755,22 +808,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -778,59 +816,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -852,38 +845,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -898,13 +891,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,7 +951,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -928,25 +981,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -964,25 +1005,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -994,73 +1029,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,7 +1047,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,6 +1090,32 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1147,36 +1160,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1190,17 +1183,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1209,148 +1196,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1722,7 +1709,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>